<commit_message>
cgap_submit_test.xlsx modified for more testing
</commit_message>
<xml_diff>
--- a/src/encoded/tests/data/documents/cgap_submit_test.xlsx
+++ b/src/encoded/tests/data/documents/cgap_submit_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/cgap-portal/src/encoded/tests/data/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21686A8A-DF93-D248-9254-0B7C04ADAB54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A186957D-9B1A-0443-9ED0-F048203729CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="3500" windowWidth="26780" windowHeight="13080" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
+    <workbookView xWindow="5040" yWindow="3500" windowWidth="32060" windowHeight="14860" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Accession data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="90">
   <si>
     <t>Other ID</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>Sample ID</t>
+  </si>
+  <si>
+    <t>Analysis ID</t>
   </si>
 </sst>
 </file>
@@ -472,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -542,6 +545,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -878,85 +887,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23985C4D-01B8-468F-8F7A-3E2DDE3ABF1C}">
-  <dimension ref="A1:BZ6"/>
+  <dimension ref="A1:CA6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AJ3" sqref="AJ3"/>
+      <selection activeCell="AE6" sqref="AE6:AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.6640625" style="6" customWidth="1"/>
-    <col min="2" max="8" width="12.6640625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="30" customWidth="1"/>
-    <col min="11" max="18" width="16" style="9" customWidth="1"/>
-    <col min="19" max="19" width="14.5" style="6" customWidth="1"/>
-    <col min="20" max="20" width="15.5" style="6" customWidth="1"/>
-    <col min="21" max="21" width="14.33203125" style="6" customWidth="1"/>
-    <col min="22" max="22" width="16.5" style="6" customWidth="1"/>
-    <col min="23" max="23" width="12.6640625" style="8" customWidth="1"/>
-    <col min="24" max="33" width="16" style="9" customWidth="1"/>
-    <col min="34" max="35" width="14.5" style="6" customWidth="1"/>
-    <col min="36" max="36" width="15.5" style="6" customWidth="1"/>
-    <col min="37" max="37" width="14.33203125" style="6" customWidth="1"/>
-    <col min="38" max="38" width="12.6640625" style="8" customWidth="1"/>
-    <col min="39" max="74" width="16" style="9" customWidth="1"/>
-    <col min="75" max="75" width="14.5" style="6" customWidth="1"/>
-    <col min="76" max="76" width="15.5" style="6" customWidth="1"/>
-    <col min="77" max="77" width="14.33203125" style="6" customWidth="1"/>
-    <col min="78" max="78" width="16.5" style="6" customWidth="1"/>
-    <col min="79" max="16384" width="9.1640625" style="10"/>
+    <col min="2" max="9" width="12.6640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" style="30" customWidth="1"/>
+    <col min="12" max="19" width="16" style="9" customWidth="1"/>
+    <col min="20" max="20" width="14.5" style="6" customWidth="1"/>
+    <col min="21" max="21" width="15.5" style="6" customWidth="1"/>
+    <col min="22" max="22" width="14.33203125" style="6" customWidth="1"/>
+    <col min="23" max="23" width="16.5" style="6" customWidth="1"/>
+    <col min="24" max="24" width="12.6640625" style="8" customWidth="1"/>
+    <col min="25" max="34" width="16" style="9" customWidth="1"/>
+    <col min="35" max="36" width="14.5" style="6" customWidth="1"/>
+    <col min="37" max="37" width="15.5" style="6" customWidth="1"/>
+    <col min="38" max="38" width="14.33203125" style="6" customWidth="1"/>
+    <col min="39" max="39" width="12.6640625" style="8" customWidth="1"/>
+    <col min="40" max="75" width="16" style="9" customWidth="1"/>
+    <col min="76" max="76" width="14.5" style="6" customWidth="1"/>
+    <col min="77" max="77" width="15.5" style="6" customWidth="1"/>
+    <col min="78" max="78" width="14.33203125" style="6" customWidth="1"/>
+    <col min="79" max="79" width="16.5" style="6" customWidth="1"/>
+    <col min="80" max="16384" width="9.1640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" s="5" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:79" s="5" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="34" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="31" t="s">
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="34" t="s">
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="25"/>
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="34"/>
+      <c r="AC1" s="34"/>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="34"/>
+      <c r="AI1" s="34"/>
+      <c r="AJ1" s="34"/>
+      <c r="AK1" s="34"/>
+      <c r="AL1" s="34"/>
+      <c r="AM1" s="35"/>
       <c r="AN1" s="25"/>
       <c r="AO1" s="25"/>
       <c r="AP1" s="25"/>
@@ -992,12 +1001,13 @@
       <c r="BT1" s="25"/>
       <c r="BU1" s="25"/>
       <c r="BV1" s="25"/>
-      <c r="BW1" s="26"/>
+      <c r="BW1" s="25"/>
       <c r="BX1" s="26"/>
       <c r="BY1" s="26"/>
       <c r="BZ1" s="26"/>
+      <c r="CA1" s="26"/>
     </row>
-    <row r="2" spans="1:78" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:79" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>84</v>
       </c>
@@ -1022,97 +1032,99 @@
       <c r="H2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="K2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="L2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="M2" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="N2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="O2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="P2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="Q2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="R2" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="S2" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="T2" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="T2" s="18" t="s">
+      <c r="U2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="18" t="s">
+      <c r="V2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="18" t="s">
+      <c r="W2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="19" t="s">
+      <c r="X2" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="X2" s="22" t="s">
+      <c r="Y2" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="Y2" s="22" t="s">
+      <c r="Z2" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="Z2" s="22" t="s">
+      <c r="AA2" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="AA2" s="22" t="s">
+      <c r="AB2" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="AB2" s="22" t="s">
+      <c r="AC2" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="AC2" s="22" t="s">
+      <c r="AD2" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="AD2" s="22" t="s">
+      <c r="AE2" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="AE2" s="22" t="s">
+      <c r="AF2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="AF2" s="22" t="s">
+      <c r="AG2" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="AG2" s="22" t="s">
+      <c r="AH2" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="AH2" s="22" t="s">
+      <c r="AI2" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="AI2" s="22" t="s">
+      <c r="AJ2" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="AJ2" s="22" t="s">
+      <c r="AK2" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="AK2" s="22" t="s">
+      <c r="AL2" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AM2" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="AM2" s="4"/>
       <c r="AN2" s="4"/>
       <c r="AO2" s="4"/>
       <c r="AP2" s="4"/>
@@ -1148,12 +1160,13 @@
       <c r="BT2" s="4"/>
       <c r="BU2" s="4"/>
       <c r="BV2" s="4"/>
-      <c r="BW2" s="2"/>
+      <c r="BW2" s="4"/>
       <c r="BX2" s="2"/>
       <c r="BY2" s="2"/>
       <c r="BZ2" s="2"/>
+      <c r="CA2" s="2"/>
     </row>
-    <row r="3" spans="1:78" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:79" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>73</v>
       </c>
@@ -1176,89 +1189,89 @@
       <c r="H3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="17" t="s">
+      <c r="I3" s="32"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="M3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="N3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="O3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="P3" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="Q3" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="R3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="17" t="s">
+      <c r="S3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="S3" s="17" t="s">
+      <c r="T3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="T3" s="20" t="s">
+      <c r="U3" s="20" t="s">
         <v>27</v>
-      </c>
-      <c r="U3" s="20" t="s">
-        <v>5</v>
       </c>
       <c r="V3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="W3" s="21" t="s">
+      <c r="W3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="X3" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AD3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AF3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AG3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AH3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AH3" s="1" t="s">
+      <c r="AI3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AI3" s="1" t="s">
+      <c r="AJ3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AJ3" s="24" t="s">
+      <c r="AK3" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="AK3" s="1" t="s">
+      <c r="AL3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AM3" s="12"/>
       <c r="AN3" s="12"/>
       <c r="AO3" s="12"/>
       <c r="AP3" s="12"/>
@@ -1294,8 +1307,9 @@
       <c r="BT3" s="12"/>
       <c r="BU3" s="12"/>
       <c r="BV3" s="12"/>
+      <c r="BW3" s="12"/>
     </row>
-    <row r="4" spans="1:78" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:79" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
         <v>456</v>
       </c>
@@ -1316,72 +1330,75 @@
       <c r="H4" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="17" t="s">
+      <c r="I4" s="32">
+        <v>55432</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="L4" s="28">
+      <c r="M4" s="28">
         <v>43863</v>
       </c>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17">
+      <c r="N4" s="17"/>
+      <c r="O4" s="17">
         <v>11946744</v>
       </c>
-      <c r="O4" s="17" t="s">
+      <c r="P4" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="17" t="s">
+      <c r="Q4" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="Q4" s="28">
+      <c r="R4" s="28">
         <v>43892</v>
       </c>
-      <c r="R4" s="17" t="s">
+      <c r="S4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="S4" s="17" t="s">
+      <c r="T4" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="T4" s="20" t="s">
+      <c r="U4" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="U4" s="20"/>
       <c r="V4" s="20"/>
-      <c r="W4" s="21"/>
-      <c r="X4" s="1">
+      <c r="W4" s="20"/>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="1">
         <v>3464467</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AB4" s="23">
+      <c r="AC4" s="23">
         <v>44137</v>
       </c>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="23">
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="23">
         <v>44137</v>
       </c>
-      <c r="AE4" s="23" t="s">
+      <c r="AF4" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AG4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AG4" s="1" t="s">
+      <c r="AH4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
-      <c r="AK4" s="24"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="24"/>
     </row>
-    <row r="5" spans="1:78" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:79" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="14">
         <v>789</v>
       </c>
@@ -1402,8 +1419,66 @@
       <c r="H5" s="14" t="s">
         <v>11</v>
       </c>
+      <c r="I5" s="32">
+        <v>55432</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="M5" s="28">
+        <v>43863</v>
+      </c>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17">
+        <v>11946744</v>
+      </c>
+      <c r="P5" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" s="28">
+        <v>43892</v>
+      </c>
+      <c r="S5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="T5" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="U5" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="V5" s="20"/>
+      <c r="W5" s="20"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="1">
+        <v>3464468</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC5" s="23">
+        <v>44137</v>
+      </c>
+      <c r="AE5" s="23">
+        <v>44137</v>
+      </c>
+      <c r="AF5" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="6" spans="1:78" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:79" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
         <v>123</v>
       </c>
@@ -1424,13 +1499,71 @@
       <c r="H6" s="14" t="s">
         <v>11</v>
       </c>
+      <c r="I6" s="32">
+        <v>55432</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="M6" s="28">
+        <v>43863</v>
+      </c>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17">
+        <v>11946744</v>
+      </c>
+      <c r="P6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q6" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="R6" s="28">
+        <v>43892</v>
+      </c>
+      <c r="S6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="T6" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="U6" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="V6" s="20"/>
+      <c r="W6" s="20"/>
+      <c r="X6" s="21"/>
+      <c r="Y6" s="1">
+        <v>3464469</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC6" s="23">
+        <v>44137</v>
+      </c>
+      <c r="AE6" s="23">
+        <v>44137</v>
+      </c>
+      <c r="AF6" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="T1:W1"/>
-    <mergeCell ref="X1:AL1"/>
-    <mergeCell ref="J1:S1"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="U1:X1"/>
+    <mergeCell ref="Y1:AM1"/>
+    <mergeCell ref="K1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
edits to tests for submit.py
</commit_message>
<xml_diff>
--- a/src/encoded/tests/data/documents/cgap_submit_test.xlsx
+++ b/src/encoded/tests/data/documents/cgap_submit_test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/cgap-portal/src/encoded/tests/data/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A186957D-9B1A-0443-9ED0-F048203729CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2300D089-AFEE-034F-8E5F-D04FF10242E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5040" yWindow="3500" windowWidth="32060" windowHeight="14860" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
   </bookViews>
@@ -279,9 +279,6 @@
     <t>Specimen Notes</t>
   </si>
   <si>
-    <t>Patient ID</t>
-  </si>
-  <si>
     <t>Family ID</t>
   </si>
   <si>
@@ -295,6 +292,9 @@
   </si>
   <si>
     <t>Analysis ID</t>
+  </si>
+  <si>
+    <t>Individual ID</t>
   </si>
 </sst>
 </file>
@@ -890,7 +890,7 @@
   <dimension ref="A1:CA6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AE6" sqref="AE6:AH6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1009,16 +1009,16 @@
     </row>
     <row r="2" spans="1:79" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>84</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>76</v>
@@ -1033,13 +1033,13 @@
         <v>2</v>
       </c>
       <c r="I2" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>81</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L2" s="16" t="s">
         <v>16</v>
@@ -1117,7 +1117,7 @@
         <v>71</v>
       </c>
       <c r="AK2" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AL2" s="22" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
added files column to submit test workbook
</commit_message>
<xml_diff>
--- a/src/encoded/tests/data/documents/cgap_submit_test.xlsx
+++ b/src/encoded/tests/data/documents/cgap_submit_test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/cgap-portal/src/encoded/tests/data/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2300D089-AFEE-034F-8E5F-D04FF10242E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896E8EB2-B3B0-6241-A958-B22D0B0DA377}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5040" yWindow="3500" windowWidth="32060" windowHeight="14860" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="94">
   <si>
     <t>Other ID</t>
   </si>
@@ -295,6 +295,18 @@
   </si>
   <si>
     <t>Individual ID</t>
+  </si>
+  <si>
+    <t>Files</t>
+  </si>
+  <si>
+    <t>f1.fastq.gz, f2.fastq.gz</t>
+  </si>
+  <si>
+    <t>f3.fastq.gz</t>
+  </si>
+  <si>
+    <t>f4.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -475,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -566,6 +578,11 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -887,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23985C4D-01B8-468F-8F7A-3E2DDE3ABF1C}">
-  <dimension ref="A1:CA6"/>
+  <dimension ref="A1:CB6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="AM13" sqref="AM13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -909,16 +926,17 @@
     <col min="35" max="36" width="14.5" style="6" customWidth="1"/>
     <col min="37" max="37" width="15.5" style="6" customWidth="1"/>
     <col min="38" max="38" width="14.33203125" style="6" customWidth="1"/>
-    <col min="39" max="39" width="12.6640625" style="8" customWidth="1"/>
-    <col min="40" max="75" width="16" style="9" customWidth="1"/>
-    <col min="76" max="76" width="14.5" style="6" customWidth="1"/>
-    <col min="77" max="77" width="15.5" style="6" customWidth="1"/>
-    <col min="78" max="78" width="14.33203125" style="6" customWidth="1"/>
-    <col min="79" max="79" width="16.5" style="6" customWidth="1"/>
-    <col min="80" max="16384" width="9.1640625" style="10"/>
+    <col min="39" max="39" width="14.33203125" style="7" customWidth="1"/>
+    <col min="40" max="40" width="12.6640625" style="8" customWidth="1"/>
+    <col min="41" max="76" width="16" style="9" customWidth="1"/>
+    <col min="77" max="77" width="14.5" style="6" customWidth="1"/>
+    <col min="78" max="78" width="15.5" style="6" customWidth="1"/>
+    <col min="79" max="79" width="14.33203125" style="6" customWidth="1"/>
+    <col min="80" max="80" width="16.5" style="6" customWidth="1"/>
+    <col min="81" max="16384" width="9.1640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79" s="5" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:80" s="5" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>15</v>
       </c>
@@ -965,8 +983,8 @@
       <c r="AJ1" s="34"/>
       <c r="AK1" s="34"/>
       <c r="AL1" s="34"/>
-      <c r="AM1" s="35"/>
-      <c r="AN1" s="25"/>
+      <c r="AM1" s="34"/>
+      <c r="AN1" s="35"/>
       <c r="AO1" s="25"/>
       <c r="AP1" s="25"/>
       <c r="AQ1" s="25"/>
@@ -1002,12 +1020,13 @@
       <c r="BU1" s="25"/>
       <c r="BV1" s="25"/>
       <c r="BW1" s="25"/>
-      <c r="BX1" s="26"/>
+      <c r="BX1" s="25"/>
       <c r="BY1" s="26"/>
       <c r="BZ1" s="26"/>
       <c r="CA1" s="26"/>
+      <c r="CB1" s="26"/>
     </row>
-    <row r="2" spans="1:79" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:80" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>89</v>
       </c>
@@ -1122,10 +1141,12 @@
       <c r="AL2" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AM2" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="AN2" s="4"/>
+      <c r="AN2" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="AO2" s="4"/>
       <c r="AP2" s="4"/>
       <c r="AQ2" s="4"/>
@@ -1161,12 +1182,13 @@
       <c r="BU2" s="4"/>
       <c r="BV2" s="4"/>
       <c r="BW2" s="4"/>
-      <c r="BX2" s="2"/>
+      <c r="BX2" s="4"/>
       <c r="BY2" s="2"/>
       <c r="BZ2" s="2"/>
       <c r="CA2" s="2"/>
+      <c r="CB2" s="2"/>
     </row>
-    <row r="3" spans="1:79" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:80" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>73</v>
       </c>
@@ -1272,7 +1294,7 @@
       <c r="AL3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AN3" s="12"/>
+      <c r="AM3" s="39"/>
       <c r="AO3" s="12"/>
       <c r="AP3" s="12"/>
       <c r="AQ3" s="12"/>
@@ -1308,8 +1330,9 @@
       <c r="BU3" s="12"/>
       <c r="BV3" s="12"/>
       <c r="BW3" s="12"/>
+      <c r="BX3" s="12"/>
     </row>
-    <row r="4" spans="1:79" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:80" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
         <v>456</v>
       </c>
@@ -1397,8 +1420,12 @@
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="24"/>
+      <c r="AM4" s="40"/>
+      <c r="AN4" s="8" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="5" spans="1:79" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:80" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="14">
         <v>789</v>
       </c>
@@ -1477,8 +1504,11 @@
       <c r="AH5" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="AN5" s="8" t="s">
+        <v>92</v>
+      </c>
     </row>
-    <row r="6" spans="1:79" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:80" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
         <v>123</v>
       </c>
@@ -1557,12 +1587,15 @@
       <c r="AH6" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="AN6" s="8" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="U1:X1"/>
-    <mergeCell ref="Y1:AM1"/>
+    <mergeCell ref="Y1:AN1"/>
     <mergeCell ref="K1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update tests and fix ValueError for bad cells
</commit_message>
<xml_diff>
--- a/src/encoded/tests/data/documents/cgap_submit_test.xlsx
+++ b/src/encoded/tests/data/documents/cgap_submit_test.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/cgap-portal/src/encoded/tests/data/documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/cgap-portal/src/encoded/tests/data/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896E8EB2-B3B0-6241-A958-B22D0B0DA377}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352F55F3-6303-C141-9452-788764ACCA60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="3500" windowWidth="32060" windowHeight="14860" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
+    <workbookView xWindow="680" yWindow="1900" windowWidth="28800" windowHeight="14860" activeTab="1" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Accession data" sheetId="1" r:id="rId1"/>
+    <sheet name="Ignored" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="94">
   <si>
     <t>Other ID</t>
   </si>
@@ -563,6 +564,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -578,11 +584,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -906,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23985C4D-01B8-468F-8F7A-3E2DDE3ABF1C}">
   <dimension ref="A1:CB6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AM13" sqref="AM13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -937,54 +938,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:80" s="5" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="36" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="33" t="s">
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="36" t="s">
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="35"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="38"/>
       <c r="AO1" s="25"/>
       <c r="AP1" s="25"/>
       <c r="AQ1" s="25"/>
@@ -1141,7 +1142,7 @@
       <c r="AL2" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AM2" s="38" t="s">
+      <c r="AM2" s="33" t="s">
         <v>83</v>
       </c>
       <c r="AN2" s="3" t="s">
@@ -1294,7 +1295,7 @@
       <c r="AL3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AM3" s="39"/>
+      <c r="AM3" s="34"/>
       <c r="AO3" s="12"/>
       <c r="AP3" s="12"/>
       <c r="AQ3" s="12"/>
@@ -1420,7 +1421,7 @@
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="24"/>
-      <c r="AM4" s="40"/>
+      <c r="AM4" s="35"/>
       <c r="AN4" s="8" t="s">
         <v>91</v>
       </c>
@@ -1601,4 +1602,120 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A6650E-94D8-DA43-955A-5D2FDE588FE0}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="38"/>
+    </row>
+    <row r="2" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="14">
+        <v>459</v>
+      </c>
+      <c r="B4" s="14">
+        <v>334</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="27">
+        <v>1990</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="32">
+        <v>55439</v>
+      </c>
+      <c r="J4" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Drr submit openpyxl (#370)
* Replace xlrd with openpyxl for submit.py

Update submit.py and associated tests to use openpyxl. Note: .xls files
no longer acceptable for case submissions.

* Bump version and fix test bug

* Fix test

* Fix dependency issue

* Add float to int coverage

* Remove xlrd and xlreader.py

* Remove xlwt package

* Update tests and fix ValueError for bad cells
</commit_message>
<xml_diff>
--- a/src/encoded/tests/data/documents/cgap_submit_test.xlsx
+++ b/src/encoded/tests/data/documents/cgap_submit_test.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/cgap-portal/src/encoded/tests/data/documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/cgap-portal/src/encoded/tests/data/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896E8EB2-B3B0-6241-A958-B22D0B0DA377}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352F55F3-6303-C141-9452-788764ACCA60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="3500" windowWidth="32060" windowHeight="14860" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
+    <workbookView xWindow="680" yWindow="1900" windowWidth="28800" windowHeight="14860" activeTab="1" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Accession data" sheetId="1" r:id="rId1"/>
+    <sheet name="Ignored" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="94">
   <si>
     <t>Other ID</t>
   </si>
@@ -563,6 +564,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -578,11 +584,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -906,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23985C4D-01B8-468F-8F7A-3E2DDE3ABF1C}">
   <dimension ref="A1:CB6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AM13" sqref="AM13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -937,54 +938,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:80" s="5" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="36" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="33" t="s">
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="36" t="s">
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="35"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="38"/>
       <c r="AO1" s="25"/>
       <c r="AP1" s="25"/>
       <c r="AQ1" s="25"/>
@@ -1141,7 +1142,7 @@
       <c r="AL2" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="AM2" s="38" t="s">
+      <c r="AM2" s="33" t="s">
         <v>83</v>
       </c>
       <c r="AN2" s="3" t="s">
@@ -1294,7 +1295,7 @@
       <c r="AL3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AM3" s="39"/>
+      <c r="AM3" s="34"/>
       <c r="AO3" s="12"/>
       <c r="AP3" s="12"/>
       <c r="AQ3" s="12"/>
@@ -1420,7 +1421,7 @@
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="24"/>
-      <c r="AM4" s="40"/>
+      <c r="AM4" s="35"/>
       <c r="AN4" s="8" t="s">
         <v>91</v>
       </c>
@@ -1601,4 +1602,120 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A6650E-94D8-DA43-955A-5D2FDE588FE0}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="38"/>
+    </row>
+    <row r="2" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="14">
+        <v>459</v>
+      </c>
+      <c r="B4" s="14">
+        <v>334</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="27">
+        <v>1990</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="32">
+        <v>55439</v>
+      </c>
+      <c r="J4" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove files from test workbook
</commit_message>
<xml_diff>
--- a/src/encoded/tests/data/documents/cgap_submit_test.xlsx
+++ b/src/encoded/tests/data/documents/cgap_submit_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/cgap-portal/src/encoded/tests/data/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352F55F3-6303-C141-9452-788764ACCA60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0D6B88-72B1-7141-A59A-C0D7658F045B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1900" windowWidth="28800" windowHeight="14860" activeTab="1" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
+    <workbookView xWindow="0" yWindow="1900" windowWidth="28800" windowHeight="14860" xr2:uid="{FB0E66EA-1423-4875-8AFB-50DDC911B1EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Accession data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="91">
   <si>
     <t>Other ID</t>
   </si>
@@ -299,15 +299,6 @@
   </si>
   <si>
     <t>Files</t>
-  </si>
-  <si>
-    <t>f1.fastq.gz, f2.fastq.gz</t>
-  </si>
-  <si>
-    <t>f3.fastq.gz</t>
-  </si>
-  <si>
-    <t>f4.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -907,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23985C4D-01B8-468F-8F7A-3E2DDE3ABF1C}">
   <dimension ref="A1:CB6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:J4"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AN4" sqref="AN4:AN6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1422,9 +1413,6 @@
       <c r="AK4" s="1"/>
       <c r="AL4" s="24"/>
       <c r="AM4" s="35"/>
-      <c r="AN4" s="8" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="5" spans="1:80" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="14">
@@ -1505,9 +1493,6 @@
       <c r="AH5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AN5" s="8" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="6" spans="1:80" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
@@ -1587,9 +1572,6 @@
       </c>
       <c r="AH6" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="AN6" s="8" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1608,7 +1590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A6650E-94D8-DA43-955A-5D2FDE588FE0}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>

</xml_diff>